<commit_message>
commiting IBG Cao Scripts - Sarib Shamim
</commit_message>
<xml_diff>
--- a/Data/CCSameDayInputter.xlsx
+++ b/Data/CCSameDayInputter.xlsx
@@ -12,12 +12,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Transaction Number</t>
   </si>
   <si>
     <t>BKAC2300600141</t>
+  </si>
+  <si>
+    <t>BKAC2300900001</t>
   </si>
 </sst>
 </file>
@@ -62,7 +65,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -78,6 +81,11 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>